<commit_message>
rerun and summarise models without urban landuse
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/carown_LR/Berlin.xlsx
+++ b/outputs/ML_Results/carown_LR/Berlin.xlsx
@@ -7,15 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summ37" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="summ6" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="summ3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="summ1" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="summ0" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="summ2" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="summ4" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="summ11" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="summ7" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="summ3" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="summ11" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="summ4" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="summ2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="summ6" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="summ8" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="summ27" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="summ0" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="summ1" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,10 +466,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.874744465790519</v>
+        <v>-2.08758573962203</v>
       </c>
       <c r="C2" t="n">
-        <v>3.219994118626095e-06</v>
+        <v>2.070281016918037e-07</v>
       </c>
     </row>
     <row r="3">
@@ -479,10 +479,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1945230289869524</v>
+        <v>0.1280517145965852</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02817667052438058</v>
+        <v>0.1536222647523187</v>
       </c>
     </row>
     <row r="4">
@@ -492,257 +492,244 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.147586800183331</v>
+        <v>-1.135525432725436</v>
       </c>
       <c r="C4" t="n">
-        <v>6.401245239205685e-51</v>
+        <v>1.112925446165808e-49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female_Parent]</t>
+          <t>HHType_simp[T.Single_Male]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.05042796798161264</v>
+        <v>-0.7180588471788427</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6750138857491622</v>
+        <v>2.788906249457725e-19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>HHType_simp[T.Single_Parent]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.7467061709476057</v>
+        <v>-0.1906721770090037</v>
       </c>
       <c r="C6" t="n">
-        <v>8.193578949999496e-21</v>
+        <v>0.08627535983745159</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male_Parent]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.7688354735253845</v>
+        <v>0.08729348493177912</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00576846123211238</v>
+        <v>0.04420790976073428</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.05164969963939398</v>
+        <v>0.0002926407321361216</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2264241055354849</v>
+        <v>8.869769981590212e-61</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0002894622970047212</v>
+        <v>0.02041412677479729</v>
       </c>
       <c r="C9" t="n">
-        <v>1.215189945778005e-59</v>
+        <v>3.251741834761878e-28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01919680181347679</v>
+        <v>-0.2061059760309263</v>
       </c>
       <c r="C10" t="n">
-        <v>2.434630916730311e-25</v>
+        <v>5.528632080973405e-05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.1845066377664023</v>
+        <v>0.3749446217009432</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0003210604971529639</v>
+        <v>3.51757671283141e-06</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.4663234574081544</v>
+        <v>0.3324608256274597</v>
       </c>
       <c r="C12" t="n">
-        <v>7.843730723409847e-09</v>
+        <v>0.0008022281008840093</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.4144989981325921</v>
+        <v>-7.141696400858087e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>2.784117826166486e-05</v>
+        <v>1.050793029453501e-22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>UrbBuildDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-7.342236765553442e-05</v>
+        <v>7.919600530722134e-09</v>
       </c>
       <c r="C14" t="n">
-        <v>4.702525860348821e-24</v>
+        <v>0.4859285750577185</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3.661392318948989e-09</v>
+        <v>0.0005382747494799024</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7481283221713872</v>
+        <v>0.9737329244433095</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.01182581948812293</v>
+        <v>0.07958105099353503</v>
       </c>
       <c r="C16" t="n">
-        <v>0.4730624090820263</v>
+        <v>1.634447829757925e-17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07766622253995324</v>
+        <v>-0.3651493059249178</v>
       </c>
       <c r="C17" t="n">
-        <v>7.561283359342512e-17</v>
+        <v>0.3537307931342428</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>bike_lane_share</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.2219983006107909</v>
+        <v>0.001109851852830426</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5741146535041917</v>
+        <v>0.696573587323585</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IntersecDensity</t>
+          <t>StreetLength</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>4.816779748544101e-05</v>
+        <v>0.002595247823327394</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9865620107074473</v>
+        <v>0.09307070857268054</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.001794949273849506</v>
+        <v>1.164709522407536</v>
       </c>
       <c r="C20" t="n">
-        <v>0.24795084271798</v>
+        <v>1.039167723555255e-06</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LU_UrbFab</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.170368964074879</v>
+        <v>-0.1724172932812966</v>
       </c>
       <c r="C21" t="n">
-        <v>9.447961466490659e-07</v>
+        <v>0.5674354858133417</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LU_Comm</t>
+          <t>LU_Urban</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.2283182635206542</v>
+        <v>-0.4161027272852567</v>
       </c>
       <c r="C22" t="n">
-        <v>0.4475806509127347</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-0.4100015789121185</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.05778416522207554</v>
+        <v>0.05424491704269578</v>
       </c>
     </row>
   </sheetData>
@@ -756,7 +743,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -788,10 +775,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.979638722527581</v>
+        <v>-2.082832846812584</v>
       </c>
       <c r="C2" t="n">
-        <v>8.388886578157498e-07</v>
+        <v>1.833341490357055e-07</v>
       </c>
     </row>
     <row r="3">
@@ -801,10 +788,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1976597313138327</v>
+        <v>0.1530801298630984</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02530607885580519</v>
+        <v>0.08481474599516155</v>
       </c>
     </row>
     <row r="4">
@@ -814,257 +801,244 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.192835754282042</v>
+        <v>-1.175483005935532</v>
       </c>
       <c r="C4" t="n">
-        <v>7.149093098072149e-55</v>
+        <v>2.910354592986776e-53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female_Parent]</t>
+          <t>HHType_simp[T.Single_Male]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.1416204810405239</v>
+        <v>-0.7264697937806168</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2403297183359689</v>
+        <v>1.097426557372159e-19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>HHType_simp[T.Single_Parent]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.7179159137496213</v>
+        <v>-0.1940762801218127</v>
       </c>
       <c r="C6" t="n">
-        <v>1.911013519858915e-19</v>
+        <v>0.08356243776495302</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male_Parent]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.8044182602809477</v>
+        <v>0.06722323415944671</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00251876208117933</v>
+        <v>0.1196171167574819</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.05338291439654053</v>
+        <v>0.0002782781070856956</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2101896998878426</v>
+        <v>2.007195865076835e-55</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0002871224765281146</v>
+        <v>0.01960874951943636</v>
       </c>
       <c r="C9" t="n">
-        <v>7.928240709408228e-59</v>
+        <v>1.744864357214495e-26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.02059022807553994</v>
+        <v>-0.1664107630533422</v>
       </c>
       <c r="C10" t="n">
-        <v>1.006531052470962e-28</v>
+        <v>0.001125157911111269</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.2015114272914474</v>
+        <v>0.4058448968614469</v>
       </c>
       <c r="C11" t="n">
-        <v>8.268116348623614e-05</v>
+        <v>4.131788734638135e-07</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3930478259400223</v>
+        <v>0.3418067826769314</v>
       </c>
       <c r="C12" t="n">
-        <v>1.332384942938661e-06</v>
+        <v>0.000513903275130259</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3311886409321831</v>
+        <v>-7.332474611415027e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0008146705347482316</v>
+        <v>5.012886850831805e-24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>UrbBuildDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-6.708439715216967e-05</v>
+        <v>4.311469831398117e-09</v>
       </c>
       <c r="C14" t="n">
-        <v>1.712088289757287e-20</v>
+        <v>0.7054412197187698</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-4.833326627917499e-09</v>
+        <v>0.006870342247563254</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6686660891796816</v>
+        <v>0.6701733830826047</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.001494457389042797</v>
+        <v>0.07359770359897745</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9265551288092984</v>
+        <v>1.878362222031774e-15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07634012162271156</v>
+        <v>-0.3814087285159948</v>
       </c>
       <c r="C17" t="n">
-        <v>1.944150969196797e-16</v>
+        <v>0.3321546363105182</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>bike_lane_share</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.3001849636767636</v>
+        <v>0.002783923003090526</v>
       </c>
       <c r="C18" t="n">
-        <v>0.4475410750824396</v>
+        <v>0.3280268762000876</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IntersecDensity</t>
+          <t>StreetLength</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.002173941828110272</v>
+        <v>0.003350249551987248</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4467693543543508</v>
+        <v>0.03140437615670362</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.00266344988387939</v>
+        <v>1.08511933604872</v>
       </c>
       <c r="C20" t="n">
-        <v>0.08797951280542424</v>
+        <v>4.985538748800539e-06</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LU_UrbFab</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.146870969737662</v>
+        <v>-0.1328858987692287</v>
       </c>
       <c r="C21" t="n">
-        <v>1.406373886652353e-06</v>
+        <v>0.6569492037467328</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LU_Comm</t>
+          <t>LU_Urban</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2.670631330546143e-05</v>
+        <v>-0.4000623058994169</v>
       </c>
       <c r="C22" t="n">
-        <v>0.9999290785897822</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-0.5005254709183117</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.02029331280161339</v>
+        <v>0.06284848039272241</v>
       </c>
     </row>
   </sheetData>
@@ -1078,7 +1052,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1110,10 +1084,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.921101780335632</v>
+        <v>-1.980369403495468</v>
       </c>
       <c r="C2" t="n">
-        <v>1.785085291313266e-06</v>
+        <v>8.179228347947119e-07</v>
       </c>
     </row>
     <row r="3">
@@ -1123,10 +1097,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1029778474115502</v>
+        <v>0.125939328570613</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2480012803948027</v>
+        <v>0.154537659384375</v>
       </c>
     </row>
     <row r="4">
@@ -1136,257 +1110,244 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.173441363761827</v>
+        <v>-1.168039847871428</v>
       </c>
       <c r="C4" t="n">
-        <v>3.718861106896655e-53</v>
+        <v>2.699410652468072e-52</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female_Parent]</t>
+          <t>HHType_simp[T.Single_Male]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.1973931276511965</v>
+        <v>-0.7625617387850488</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0977034516663802</v>
+        <v>1.455942268475826e-21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>HHType_simp[T.Single_Parent]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.8015884091718786</v>
+        <v>-0.2141403734356452</v>
       </c>
       <c r="C6" t="n">
-        <v>1.018816158474546e-23</v>
+        <v>0.05071421129206916</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male_Parent]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.6437630910327556</v>
+        <v>0.07939293848172695</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01427577793086335</v>
+        <v>0.06258017033889687</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.06489371507535331</v>
+        <v>0.0002843314878919213</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1315322278759838</v>
+        <v>6.571408772449514e-58</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.000289991629146035</v>
+        <v>0.01910960345934223</v>
       </c>
       <c r="C9" t="n">
-        <v>6.119119235252927e-60</v>
+        <v>5.114494861218358e-25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01900115512248519</v>
+        <v>-0.2126808565012566</v>
       </c>
       <c r="C10" t="n">
-        <v>1.05507043487322e-24</v>
+        <v>3.444416364144794e-05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.1861877890949537</v>
+        <v>0.4079014938029649</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0002746598357190051</v>
+        <v>4.970758327297609e-07</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.4211128972961187</v>
+        <v>0.3842079509342966</v>
       </c>
       <c r="C12" t="n">
-        <v>1.760989934934405e-07</v>
+        <v>0.0001067675966789129</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3637153612777779</v>
+        <v>-6.897471059616255e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0002463633858005462</v>
+        <v>1.313753400673464e-21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>UrbBuildDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-7.279283470811659e-05</v>
+        <v>-3.579835208836353e-10</v>
       </c>
       <c r="C14" t="n">
-        <v>1.196340825689027e-23</v>
+        <v>0.9747646769028557</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.778566720837549e-09</v>
+        <v>0.009870104287749881</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8749672191445896</v>
+        <v>0.549054808951698</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.0005284775690718622</v>
+        <v>0.07798750481627301</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9741059070152156</v>
+        <v>4.479632246995761e-17</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07464124381921394</v>
+        <v>-0.03445165692620997</v>
       </c>
       <c r="C17" t="n">
-        <v>1.071851974876961e-15</v>
+        <v>0.9304052254211457</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>bike_lane_share</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.1291780737003453</v>
+        <v>0.0004970265459671119</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7438822283130986</v>
+        <v>0.8614709257423259</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IntersecDensity</t>
+          <t>StreetLength</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.00155112088200262</v>
+        <v>0.002686315031499509</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5864956014637321</v>
+        <v>0.08482685823959271</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.002882951591000852</v>
+        <v>1.219262414646804</v>
       </c>
       <c r="C20" t="n">
-        <v>0.06572122885864581</v>
+        <v>3.01644443852456e-07</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LU_UrbFab</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.164295763952757</v>
+        <v>-0.1174551358523414</v>
       </c>
       <c r="C21" t="n">
-        <v>9.988203655030227e-07</v>
+        <v>0.6958678525280779</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LU_Comm</t>
+          <t>LU_Urban</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.1678945043398883</v>
+        <v>-0.4772291348141879</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5775388424191736</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-0.4647901669784999</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.0313713328309174</v>
+        <v>0.02668545084493079</v>
       </c>
     </row>
   </sheetData>
@@ -1400,7 +1361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1432,10 +1393,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-2.060957673071065</v>
+        <v>-1.816666690373179</v>
       </c>
       <c r="C2" t="n">
-        <v>3.051067867589573e-07</v>
+        <v>6.08347001360474e-06</v>
       </c>
     </row>
     <row r="3">
@@ -1445,10 +1406,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.150787243248909</v>
+        <v>0.2301654919040214</v>
       </c>
       <c r="C3" t="n">
-        <v>0.09137836369682617</v>
+        <v>0.01000263465733526</v>
       </c>
     </row>
     <row r="4">
@@ -1458,257 +1419,244 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.151777455723827</v>
+        <v>-1.188717204035874</v>
       </c>
       <c r="C4" t="n">
-        <v>4.891081346992834e-51</v>
+        <v>2.087442564568932e-54</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female_Parent]</t>
+          <t>HHType_simp[T.Single_Male]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.08398819487737168</v>
+        <v>-0.7728214068621225</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4780893448640793</v>
+        <v>2.78122466957847e-22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>HHType_simp[T.Single_Parent]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.6804722382989481</v>
+        <v>-0.1777307378335531</v>
       </c>
       <c r="C6" t="n">
-        <v>1.070428387811868e-17</v>
+        <v>0.1083660802506915</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male_Parent]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.5421988718474086</v>
+        <v>0.03536765555966251</v>
       </c>
       <c r="C7" t="n">
-        <v>0.03635132020752888</v>
+        <v>0.4113690195523469</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.07408160465423004</v>
+        <v>0.0002860018694054194</v>
       </c>
       <c r="C8" t="n">
-        <v>0.08608186279323238</v>
+        <v>1.403545953218731e-58</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0002838872947891394</v>
+        <v>0.02022241974046066</v>
       </c>
       <c r="C9" t="n">
-        <v>7.709210509551682e-58</v>
+        <v>5.4285783082028e-28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.02024279243790885</v>
+        <v>-0.1970867765963544</v>
       </c>
       <c r="C10" t="n">
-        <v>3.578948180587428e-28</v>
+        <v>0.0001120189646536636</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.1718472849154661</v>
+        <v>0.3824139978098576</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0007853586387303661</v>
+        <v>2.287462602343315e-06</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3954386369362619</v>
+        <v>0.3342321265139644</v>
       </c>
       <c r="C12" t="n">
-        <v>1.120001819438576e-06</v>
+        <v>0.000689194165828236</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3692830269832906</v>
+        <v>-7.083533136258365e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0001964690939260815</v>
+        <v>1.616840091331085e-22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>UrbBuildDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-7.038707810171954e-05</v>
+        <v>-2.79177127184325e-10</v>
       </c>
       <c r="C14" t="n">
-        <v>2.862867425415522e-22</v>
+        <v>0.9806932346932512</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5.289117735212026e-09</v>
+        <v>0.006229938493742963</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6438958936849255</v>
+        <v>0.703196911726204</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.01535098796383654</v>
+        <v>0.07037350748308487</v>
       </c>
       <c r="C16" t="n">
-        <v>0.347698782348294</v>
+        <v>3.163687083489718e-14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07316235397098525</v>
+        <v>-0.06089892406108516</v>
       </c>
       <c r="C17" t="n">
-        <v>3.057604951638934e-15</v>
+        <v>0.8772625997099474</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>bike_lane_share</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.4116724233101215</v>
+        <v>0.001320873318220603</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2898565483274107</v>
+        <v>0.6428699483159126</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IntersecDensity</t>
+          <t>StreetLength</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.001279455849954536</v>
+        <v>0.002811634931463216</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6527724874305028</v>
+        <v>0.07137061768055186</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.003369406487237787</v>
+        <v>1.28228240116853</v>
       </c>
       <c r="C20" t="n">
-        <v>0.03323558191713119</v>
+        <v>6.602710102902693e-08</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LU_UrbFab</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.107731292058881</v>
+        <v>-0.1287001683591534</v>
       </c>
       <c r="C21" t="n">
-        <v>3.083252064310945e-06</v>
+        <v>0.6692097420562358</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LU_Comm</t>
+          <t>LU_Urban</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.2657042322411067</v>
+        <v>-0.606433646386578</v>
       </c>
       <c r="C22" t="n">
-        <v>0.3759331335453018</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-0.4902255462158917</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.02261420814628537</v>
+        <v>0.004956273373604779</v>
       </c>
     </row>
   </sheetData>
@@ -1722,7 +1670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1754,10 +1702,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-2.060843655275744</v>
+        <v>-1.794549253121291</v>
       </c>
       <c r="C2" t="n">
-        <v>2.761727335452113e-07</v>
+        <v>8.223520141602711e-06</v>
       </c>
     </row>
     <row r="3">
@@ -1767,10 +1715,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1319426408025593</v>
+        <v>0.1692379898621558</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1414197160881071</v>
+        <v>0.05754087719964365</v>
       </c>
     </row>
     <row r="4">
@@ -1780,257 +1728,244 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.143990690276193</v>
+        <v>-1.135855605003109</v>
       </c>
       <c r="C4" t="n">
-        <v>2.282434661658415e-50</v>
+        <v>2.210370565941984e-49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female_Parent]</t>
+          <t>HHType_simp[T.Single_Male]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.1031632961577984</v>
+        <v>-0.6973871684494017</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3834049181881686</v>
+        <v>2.562205425488756e-18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>HHType_simp[T.Single_Parent]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.7253328752668019</v>
+        <v>-0.2100245503931333</v>
       </c>
       <c r="C6" t="n">
-        <v>1.281410301897551e-19</v>
+        <v>0.05905801060726448</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male_Parent]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.6079865622756899</v>
+        <v>0.06809643459941493</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0215991904877664</v>
+        <v>0.1158536979271145</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.07031015905058026</v>
+        <v>0.0002800863506110397</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1056265661170594</v>
+        <v>3.670249423822661e-56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0002967609123345257</v>
+        <v>0.01944898080588794</v>
       </c>
       <c r="C9" t="n">
-        <v>3.315006867927988e-62</v>
+        <v>3.728589458982922e-26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01982594124129022</v>
+        <v>-0.1666624195263811</v>
       </c>
       <c r="C10" t="n">
-        <v>5.994695112048493e-27</v>
+        <v>0.00110239792456419</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.1624705506566205</v>
+        <v>0.3722358425549728</v>
       </c>
       <c r="C11" t="n">
-        <v>0.001437558033420749</v>
+        <v>3.525988477736432e-06</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3506044940676559</v>
+        <v>0.3504514833391781</v>
       </c>
       <c r="C12" t="n">
-        <v>1.280262465863639e-05</v>
+        <v>0.0003634853296858923</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3128891171736415</v>
+        <v>-7.103961707161005e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0015301586873907</v>
+        <v>1.37820414005112e-22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>UrbBuildDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-6.825577889512742e-05</v>
+        <v>-2.841859677492108e-09</v>
       </c>
       <c r="C14" t="n">
-        <v>4.613812906906724e-21</v>
+        <v>0.8039495599870059</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6.28576044346324e-10</v>
+        <v>-0.0011641895942622</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9559819297842979</v>
+        <v>0.9430294314953924</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.007184116820775434</v>
+        <v>0.07300002912283675</v>
       </c>
       <c r="C16" t="n">
-        <v>0.6602983412300519</v>
+        <v>4.889505875285364e-15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07757254791653193</v>
+        <v>-0.136052463991979</v>
       </c>
       <c r="C17" t="n">
-        <v>7.673199982213085e-17</v>
+        <v>0.7288531258100872</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>bike_lane_share</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.2436273477331585</v>
+        <v>0.0006271235343535215</v>
       </c>
       <c r="C18" t="n">
-        <v>0.536557072593262</v>
+        <v>0.8258472036850451</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IntersecDensity</t>
+          <t>StreetLength</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.001247006814836174</v>
+        <v>0.002651733507875734</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6627045439696941</v>
+        <v>0.0930750522550893</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.002639249983123269</v>
+        <v>1.193875013125902</v>
       </c>
       <c r="C20" t="n">
-        <v>0.08887321522306878</v>
+        <v>5.182369179642809e-07</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LU_UrbFab</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.184664274475768</v>
+        <v>-0.1444825189167168</v>
       </c>
       <c r="C21" t="n">
-        <v>6.395978934167067e-07</v>
+        <v>0.630447087159941</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LU_Comm</t>
+          <t>LU_Urban</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.0109716064581322</v>
+        <v>-0.5446725871767807</v>
       </c>
       <c r="C22" t="n">
-        <v>0.9708755335816268</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-0.4350809433329064</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.04315330014080939</v>
+        <v>0.0114320604491428</v>
       </c>
     </row>
   </sheetData>
@@ -2044,7 +1979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2076,10 +2011,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.96208186037859</v>
+        <v>-1.888927677751125</v>
       </c>
       <c r="C2" t="n">
-        <v>9.628606740179821e-07</v>
+        <v>2.436035456756903e-06</v>
       </c>
     </row>
     <row r="3">
@@ -2089,10 +2024,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1710071892635902</v>
+        <v>0.1296510920848891</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0554542888490251</v>
+        <v>0.143284349133897</v>
       </c>
     </row>
     <row r="4">
@@ -2102,257 +2037,244 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.165449512753031</v>
+        <v>-1.172829019807213</v>
       </c>
       <c r="C4" t="n">
-        <v>4.321863991039508e-52</v>
+        <v>6.711062311427771e-53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female_Parent]</t>
+          <t>HHType_simp[T.Single_Male]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.15822299811985</v>
+        <v>-0.7161764356705228</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1854497532228719</v>
+        <v>2.037258010260989e-19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>HHType_simp[T.Single_Parent]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.7332422419464738</v>
+        <v>-0.191300868402096</v>
       </c>
       <c r="C6" t="n">
-        <v>4.47421675141746e-20</v>
+        <v>0.08464087126983297</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male_Parent]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.5219269221252614</v>
+        <v>0.06174046661076569</v>
       </c>
       <c r="C7" t="n">
-        <v>0.04308844933844889</v>
+        <v>0.1492230428633003</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.07170224392895343</v>
+        <v>0.0003041822219770333</v>
       </c>
       <c r="C8" t="n">
-        <v>0.09691515607407174</v>
+        <v>1.76256631343902e-65</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.000300014161896972</v>
+        <v>0.01969033950197499</v>
       </c>
       <c r="C9" t="n">
-        <v>1.209760842943036e-63</v>
+        <v>1.891960054452844e-26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01916864781677945</v>
+        <v>-0.1803390887590847</v>
       </c>
       <c r="C10" t="n">
-        <v>2.40932485810149e-25</v>
+        <v>0.0004251092400172026</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.2151790210866302</v>
+        <v>0.3764349662277631</v>
       </c>
       <c r="C11" t="n">
-        <v>2.676548946379555e-05</v>
+        <v>3.146192956943224e-06</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3459948795880073</v>
+        <v>0.3190046294090331</v>
       </c>
       <c r="C12" t="n">
-        <v>1.764102694202856e-05</v>
+        <v>0.001228195173176212</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3288663052704619</v>
+        <v>-7.810443957668597e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0008096390326893213</v>
+        <v>5.930278891807778e-27</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>UrbBuildDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-6.982132672109093e-05</v>
+        <v>8.068521925445036e-09</v>
       </c>
       <c r="C14" t="n">
-        <v>5.678487200466753e-22</v>
+        <v>0.4792810357433934</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-1.374422181549097e-10</v>
+        <v>-0.001893644499184058</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9903330494961889</v>
+        <v>0.9072001098404934</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.004178957865485204</v>
+        <v>0.07218474446448843</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7964843432029953</v>
+        <v>6.059264302247756e-15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.06831309833397275</v>
+        <v>-0.5057579655779406</v>
       </c>
       <c r="C17" t="n">
-        <v>2.070136221476701e-13</v>
+        <v>0.1974056582045028</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>bike_lane_share</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.2214209099088358</v>
+        <v>0.0004680726292803492</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5768745245070344</v>
+        <v>0.8695979419748516</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IntersecDensity</t>
+          <t>StreetLength</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.000790260629186926</v>
+        <v>0.003000982031114473</v>
       </c>
       <c r="C19" t="n">
-        <v>0.7807250966298903</v>
+        <v>0.05452577523574117</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.003808068552728475</v>
+        <v>1.301098775742336</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0149014393962398</v>
+        <v>4.67298925913626e-08</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LU_UrbFab</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.240406251065943</v>
+        <v>-0.2437019376287906</v>
       </c>
       <c r="C21" t="n">
-        <v>1.873033683936197e-07</v>
+        <v>0.4181795666283172</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LU_Comm</t>
+          <t>LU_Urban</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.1303450020598542</v>
+        <v>-0.5181449034262671</v>
       </c>
       <c r="C22" t="n">
-        <v>0.6652574954376445</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-0.5361998091309378</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.01278768667760766</v>
+        <v>0.01600691673418356</v>
       </c>
     </row>
   </sheetData>
@@ -2366,7 +2288,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2398,10 +2320,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.922843968706302</v>
+        <v>-2.035019010823263</v>
       </c>
       <c r="C2" t="n">
-        <v>1.431602899009836e-06</v>
+        <v>3.701310479736041e-07</v>
       </c>
     </row>
     <row r="3">
@@ -2411,10 +2333,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1434217560407962</v>
+        <v>0.1396942698602518</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1075594555675231</v>
+        <v>0.1178377127234301</v>
       </c>
     </row>
     <row r="4">
@@ -2424,257 +2346,244 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.145262907969806</v>
+        <v>-1.10840004529217</v>
       </c>
       <c r="C4" t="n">
-        <v>1.327497961738323e-50</v>
+        <v>9.798838113784305e-48</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female_Parent]</t>
+          <t>HHType_simp[T.Single_Male]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.1289968757749542</v>
+        <v>-0.6734511122032093</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2851486298101781</v>
+        <v>3.071722618053411e-17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>HHType_simp[T.Single_Parent]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.7340499157731497</v>
+        <v>-0.1176381313495237</v>
       </c>
       <c r="C6" t="n">
-        <v>3.817753101970014e-20</v>
+        <v>0.2910306969645816</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male_Parent]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.5101636691812637</v>
+        <v>0.07477483301901079</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06050358202491656</v>
+        <v>0.08280621429210892</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.06712254143027555</v>
+        <v>0.0002995880175045746</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1184470834760503</v>
+        <v>4.991612671812014e-63</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0002918010492161738</v>
+        <v>0.01953727218020512</v>
       </c>
       <c r="C9" t="n">
-        <v>3.954761523756126e-60</v>
+        <v>2.122181797151363e-26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01960518715443577</v>
+        <v>-0.1920240547265785</v>
       </c>
       <c r="C10" t="n">
-        <v>2.359447609326056e-26</v>
+        <v>0.0001654748146344203</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.1925651963305882</v>
+        <v>0.3977085326166064</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0001613056475866908</v>
+        <v>7.610134786594857e-07</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3559398361641101</v>
+        <v>0.3549352609957711</v>
       </c>
       <c r="C12" t="n">
-        <v>1.030164868705432e-05</v>
+        <v>0.0003041244516859464</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3144085643640901</v>
+        <v>-7.114919378757528e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>0.001433311375646213</v>
+        <v>1.321426437301633e-22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>UrbBuildDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-6.976510618415657e-05</v>
+        <v>-3.820757728360132e-10</v>
       </c>
       <c r="C14" t="n">
-        <v>7.578243715439701e-22</v>
+        <v>0.9732552975618158</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-6.269885895741913e-09</v>
+        <v>0.01654742731206471</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5842946223529396</v>
+        <v>0.3123487556565275</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.005101041739544183</v>
+        <v>0.07124617326601794</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7536965225361781</v>
+        <v>1.549570987558707e-14</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07531472516866028</v>
+        <v>-0.4045068244233698</v>
       </c>
       <c r="C17" t="n">
-        <v>4.690934373650424e-16</v>
+        <v>0.301630963149436</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>bike_lane_share</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.2137356279389254</v>
+        <v>0.001610289373250594</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5878060848882916</v>
+        <v>0.5717201132595978</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IntersecDensity</t>
+          <t>StreetLength</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.001537759754767408</v>
+        <v>0.003195818456806365</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5884032507812689</v>
+        <v>0.03973969120670891</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.00232585971156986</v>
+        <v>1.141874794418253</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1330559556889176</v>
+        <v>1.679452717331794e-06</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LU_UrbFab</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.203153034105692</v>
+        <v>-0.0892431109383999</v>
       </c>
       <c r="C21" t="n">
-        <v>4.260629612363733e-07</v>
+        <v>0.7671834404799397</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LU_Comm</t>
+          <t>LU_Urban</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.1018887194228401</v>
+        <v>-0.4880458119459786</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7346276825041197</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-0.4121963188266246</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.05478923165971364</v>
+        <v>0.02354724866871515</v>
       </c>
     </row>
   </sheetData>
@@ -2688,7 +2597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2720,10 +2629,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-2.007412726114822</v>
+        <v>-1.756318731189601</v>
       </c>
       <c r="C2" t="n">
-        <v>6.475079537204082e-07</v>
+        <v>1.244242322956687e-05</v>
       </c>
     </row>
     <row r="3">
@@ -2733,10 +2642,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1816753537656609</v>
+        <v>0.1884469115088475</v>
       </c>
       <c r="C3" t="n">
-        <v>0.04268688061465063</v>
+        <v>0.03433009385215052</v>
       </c>
     </row>
     <row r="4">
@@ -2746,257 +2655,244 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.143281883353802</v>
+        <v>-1.17217367507538</v>
       </c>
       <c r="C4" t="n">
-        <v>5.757801877145997e-50</v>
+        <v>8.562216295603887e-53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female_Parent]</t>
+          <t>HHType_simp[T.Single_Male]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.09403988206773341</v>
+        <v>-0.763192139889155</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4372460674353512</v>
+        <v>1.029127965248077e-21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>HHType_simp[T.Single_Parent]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.6993764584730667</v>
+        <v>-0.1955862652577282</v>
       </c>
       <c r="C6" t="n">
-        <v>2.452758032337774e-18</v>
+        <v>0.07711550006134077</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male_Parent]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.5049185928235391</v>
+        <v>0.0569184711178163</v>
       </c>
       <c r="C7" t="n">
-        <v>0.05325567386478441</v>
+        <v>0.1848176599364294</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.075414886026545</v>
+        <v>0.0002912845969901456</v>
       </c>
       <c r="C8" t="n">
-        <v>0.08235302536856395</v>
+        <v>1.879781322377574e-60</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0002860821124271422</v>
+        <v>0.01973451744234631</v>
       </c>
       <c r="C9" t="n">
-        <v>1.211889818933817e-58</v>
+        <v>7.950194323697211e-27</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01992411456654276</v>
+        <v>-0.1803698516697025</v>
       </c>
       <c r="C10" t="n">
-        <v>2.618724974828257e-27</v>
+        <v>0.0004328155862159895</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.1676133564118213</v>
+        <v>0.3704951616362588</v>
       </c>
       <c r="C11" t="n">
-        <v>0.001040385850381119</v>
+        <v>4.488827698066192e-06</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.4005971301174162</v>
+        <v>0.3200193241865491</v>
       </c>
       <c r="C12" t="n">
-        <v>8.399224985085413e-07</v>
+        <v>0.001215670871246287</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3562227195422172</v>
+        <v>-6.893455553048796e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0003155232016695386</v>
+        <v>1.968489939877159e-21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>UrbBuildDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-7.632649558521966e-05</v>
+        <v>-2.778471191594816e-10</v>
       </c>
       <c r="C14" t="n">
-        <v>9.92767433559796e-26</v>
+        <v>0.9803775129870815</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4.063743602316991e-09</v>
+        <v>-0.001592588594433718</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7204139658367144</v>
+        <v>0.9217874231631122</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.0007165495845049695</v>
+        <v>0.07722605622114027</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9650455983587966</v>
+        <v>1.212115704445158e-16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07476422611046081</v>
+        <v>-0.310583552603203</v>
       </c>
       <c r="C17" t="n">
-        <v>8.131492372889911e-16</v>
+        <v>0.4334180190843199</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>bike_lane_share</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.3805412650393605</v>
+        <v>8.233334451837954e-05</v>
       </c>
       <c r="C18" t="n">
-        <v>0.332791049925555</v>
+        <v>0.9770462606809661</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IntersecDensity</t>
+          <t>StreetLength</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.002212269927679811</v>
+        <v>0.001883180431021225</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4378490000374667</v>
+        <v>0.2307603422727998</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.003144263132035657</v>
+        <v>1.161611245419881</v>
       </c>
       <c r="C20" t="n">
-        <v>0.04590454894693383</v>
+        <v>1.066902922562088e-06</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LU_UrbFab</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.228291739429382</v>
+        <v>-0.1614789907915427</v>
       </c>
       <c r="C21" t="n">
-        <v>2.554155226950631e-07</v>
+        <v>0.5906379258755456</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LU_Comm</t>
+          <t>LU_Urban</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.1652918155816292</v>
+        <v>-0.4833482136245835</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5825967687525229</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-0.5429582887528643</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.0118450412707503</v>
+        <v>0.02489822976560332</v>
       </c>
     </row>
   </sheetData>
@@ -3010,7 +2906,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3042,10 +2938,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.784276584271381</v>
+        <v>-1.979543335721889</v>
       </c>
       <c r="C2" t="n">
-        <v>8.313803688145323e-06</v>
+        <v>8.074449196414448e-07</v>
       </c>
     </row>
     <row r="3">
@@ -3055,10 +2951,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1150298051290832</v>
+        <v>0.1154346233662818</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1942178636920269</v>
+        <v>0.1959645114689361</v>
       </c>
     </row>
     <row r="4">
@@ -3068,257 +2964,244 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.163655277703834</v>
+        <v>-1.171615535047153</v>
       </c>
       <c r="C4" t="n">
-        <v>4.588255254022914e-52</v>
+        <v>7.732079500999084e-53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Female_Parent]</t>
+          <t>HHType_simp[T.Single_Male]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.122701957670568</v>
+        <v>-0.7442556802626554</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2971049327222116</v>
+        <v>1.246297807577603e-20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male]</t>
+          <t>HHType_simp[T.Single_Parent]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.7330783541746899</v>
+        <v>-0.2779646415119025</v>
       </c>
       <c r="C6" t="n">
-        <v>4.007460277388761e-20</v>
+        <v>0.01287009397903039</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>HHType_simp[T.Single_Male_Parent]</t>
+          <t>HHSize</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.6738418116879987</v>
+        <v>0.07673101077146259</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01181615239485883</v>
+        <v>0.07488175855641735</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HHSize</t>
+          <t>IncomeDetailed_Numeric</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.07184919349656978</v>
+        <v>0.0002904978394850484</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0944404122444121</v>
+        <v>4.233105545456869e-60</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IncomeDetailed_Numeric</t>
+          <t>maxAgeHH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0002891632702636665</v>
+        <v>0.01913260666884049</v>
       </c>
       <c r="C9" t="n">
-        <v>2.637181155561125e-59</v>
+        <v>2.674106835763898e-25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>maxAgeHH</t>
+          <t>UniversityEducation</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01985926370358481</v>
+        <v>-0.172012181102874</v>
       </c>
       <c r="C10" t="n">
-        <v>3.626918664065364e-27</v>
+        <v>0.0007643321795503141</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UniversityEducation</t>
+          <t>InEmployment</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.1960742142986403</v>
+        <v>0.377370281714108</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0001232991258134061</v>
+        <v>3.464506447382808e-06</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>InEmployment</t>
+          <t>AllRetired</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3620588730958358</v>
+        <v>0.3502760612188163</v>
       </c>
       <c r="C12" t="n">
-        <v>5.899932268023659e-06</v>
+        <v>0.0004189260666499519</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AllRetired</t>
+          <t>UrbPopDensity</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3075417773310731</v>
+        <v>-7.117257507439592e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>0.001732260645157771</v>
+        <v>1.398337953729173e-22</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>UrbPopDensity</t>
+          <t>UrbBuildDensity</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-7.564507037896181e-05</v>
+        <v>-1.787182747033854e-09</v>
       </c>
       <c r="C14" t="n">
-        <v>5.565951998723828e-25</v>
+        <v>0.8762959928811969</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>UrbBuildDensity</t>
+          <t>DistSubcenter</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.059913534289671e-08</v>
+        <v>0.006303842358572291</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3649339971367406</v>
+        <v>0.6998655336316588</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DistSubcenter</t>
+          <t>DistCenter</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.002494402625263209</v>
+        <v>0.07441240858208409</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8784425933800477</v>
+        <v>1.137336884851234e-15</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DistCenter</t>
+          <t>bike_lane_share</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.07350399271087278</v>
+        <v>-0.1489211956466299</v>
       </c>
       <c r="C17" t="n">
-        <v>2.528283831075785e-15</v>
+        <v>0.7070990225900775</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>bike_lane_share</t>
+          <t>IntersecDensity</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.201450818379125</v>
+        <v>0.002078343151569278</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6083150242359212</v>
+        <v>0.4661951112713931</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IntersecDensity</t>
+          <t>StreetLength</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>9.517942071585132e-05</v>
+        <v>0.002751239526797696</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9734006172061641</v>
+        <v>0.0782989494590115</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>LU_UrbFab</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.002603797525576367</v>
+        <v>1.225035677823444</v>
       </c>
       <c r="C20" t="n">
-        <v>0.09327130553949195</v>
+        <v>2.530480235821477e-07</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LU_UrbFab</t>
+          <t>LU_Comm</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.334152393371938</v>
+        <v>-0.07666908678146904</v>
       </c>
       <c r="C21" t="n">
-        <v>2.020779783593724e-08</v>
+        <v>0.7980821959276838</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LU_Comm</t>
+          <t>LU_Urban</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.1660505954997882</v>
+        <v>-0.484453653217824</v>
       </c>
       <c r="C22" t="n">
-        <v>0.5798704393946315</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-0.6237234637393135</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.00380921003120585</v>
+        <v>0.02427545139368116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add model of daily distance and allregion models, re run models and summary scripts
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/carown_LR/Berlin.xlsx
+++ b/outputs/ML_Results/carown_LR/Berlin.xlsx
@@ -7,15 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summ3" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="summ11" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="summ4" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="summ2" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="summ6" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="summ8" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="summ27" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="summ0" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="summ1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="summ4" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="summ8" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="summ2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="summ31" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="summ0" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="summ19" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="summ1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="summ13" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="summ14" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,10 +466,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-2.08758573962203</v>
+        <v>-2.544794348470916</v>
       </c>
       <c r="C2" t="n">
-        <v>2.070281016918037e-07</v>
+        <v>5.394367954353604e-13</v>
       </c>
     </row>
     <row r="3">
@@ -479,10 +479,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1280517145965852</v>
+        <v>0.1934115357245323</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1536222647523187</v>
+        <v>0.04172065772375115</v>
       </c>
     </row>
     <row r="4">
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.135525432725436</v>
+        <v>-1.150707207091261</v>
       </c>
       <c r="C4" t="n">
-        <v>1.112925446165808e-49</v>
+        <v>6.922538497145886e-48</v>
       </c>
     </row>
     <row r="5">
@@ -505,10 +505,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.7180588471788427</v>
+        <v>-0.5901013262327212</v>
       </c>
       <c r="C5" t="n">
-        <v>2.788906249457725e-19</v>
+        <v>6.917195038245892e-13</v>
       </c>
     </row>
     <row r="6">
@@ -518,10 +518,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.1906721770090037</v>
+        <v>-0.1796391080425902</v>
       </c>
       <c r="C6" t="n">
-        <v>0.08627535983745159</v>
+        <v>0.1119656422371123</v>
       </c>
     </row>
     <row r="7">
@@ -531,10 +531,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.08729348493177912</v>
+        <v>0.04543265848655976</v>
       </c>
       <c r="C7" t="n">
-        <v>0.04420790976073428</v>
+        <v>0.3230524991670967</v>
       </c>
     </row>
     <row r="8">
@@ -544,10 +544,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0002926407321361216</v>
+        <v>0.0003838444511156981</v>
       </c>
       <c r="C8" t="n">
-        <v>8.869769981590212e-61</v>
+        <v>3.804119749780456e-91</v>
       </c>
     </row>
     <row r="9">
@@ -557,10 +557,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.02041412677479729</v>
+        <v>0.02288693915060274</v>
       </c>
       <c r="C9" t="n">
-        <v>3.251741834761878e-28</v>
+        <v>6.440742009069619e-33</v>
       </c>
     </row>
     <row r="10">
@@ -570,10 +570,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.2061059760309263</v>
+        <v>-0.2072468789309588</v>
       </c>
       <c r="C10" t="n">
-        <v>5.528632080973405e-05</v>
+        <v>8.082807896379256e-05</v>
       </c>
     </row>
     <row r="11">
@@ -583,10 +583,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3749446217009432</v>
+        <v>0.4698847046399674</v>
       </c>
       <c r="C11" t="n">
-        <v>3.51757671283141e-06</v>
+        <v>1.081390883126009e-08</v>
       </c>
     </row>
     <row r="12">
@@ -596,10 +596,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3324608256274597</v>
+        <v>0.1529164208829709</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0008022281008840093</v>
+        <v>0.1325220009984762</v>
       </c>
     </row>
     <row r="13">
@@ -609,10 +609,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-7.141696400858087e-05</v>
+        <v>-8.247272641122999e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>1.050793029453501e-22</v>
+        <v>1.003978087548921e-28</v>
       </c>
     </row>
     <row r="14">
@@ -622,10 +622,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>7.919600530722134e-09</v>
+        <v>1.453925150862473e-08</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4859285750577185</v>
+        <v>0.186068610360949</v>
       </c>
     </row>
     <row r="15">
@@ -635,10 +635,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.0005382747494799024</v>
+        <v>0.0147274289034664</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9737329244433095</v>
+        <v>0.3638795861698503</v>
       </c>
     </row>
     <row r="16">
@@ -648,10 +648,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07958105099353503</v>
+        <v>0.08924157388707193</v>
       </c>
       <c r="C16" t="n">
-        <v>1.634447829757925e-17</v>
+        <v>2.107319326121429e-25</v>
       </c>
     </row>
     <row r="17">
@@ -661,10 +661,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.3651493059249178</v>
+        <v>-0.1792165080019861</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3537307931342428</v>
+        <v>0.6626620339483751</v>
       </c>
     </row>
     <row r="18">
@@ -674,23 +674,23 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.001109851852830426</v>
+        <v>0.001306166922332169</v>
       </c>
       <c r="C18" t="n">
-        <v>0.696573587323585</v>
+        <v>0.6578623756929323</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.002595247823327394</v>
+        <v>0.002580549955505698</v>
       </c>
       <c r="C19" t="n">
-        <v>0.09307070857268054</v>
+        <v>0.1097208540230935</v>
       </c>
     </row>
     <row r="20">
@@ -700,10 +700,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.164709522407536</v>
+        <v>1.028595176698237</v>
       </c>
       <c r="C20" t="n">
-        <v>1.039167723555255e-06</v>
+        <v>1.565444091650496e-08</v>
       </c>
     </row>
     <row r="21">
@@ -713,23 +713,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.1724172932812966</v>
+        <v>-0.6640112912867939</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5674354858133417</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.4161027272852567</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.05424491704269578</v>
+        <v>0.01450372444741125</v>
       </c>
     </row>
   </sheetData>
@@ -743,7 +730,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -775,10 +762,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-2.082832846812584</v>
+        <v>-2.492340829075087</v>
       </c>
       <c r="C2" t="n">
-        <v>1.833341490357055e-07</v>
+        <v>1.337195734491934e-12</v>
       </c>
     </row>
     <row r="3">
@@ -788,10 +775,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1530801298630984</v>
+        <v>0.2533394834342724</v>
       </c>
       <c r="C3" t="n">
-        <v>0.08481474599516155</v>
+        <v>0.008040796546925029</v>
       </c>
     </row>
     <row r="4">
@@ -801,10 +788,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.175483005935532</v>
+        <v>-1.128440331635362</v>
       </c>
       <c r="C4" t="n">
-        <v>2.910354592986776e-53</v>
+        <v>6.833022058897444e-46</v>
       </c>
     </row>
     <row r="5">
@@ -814,10 +801,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.7264697937806168</v>
+        <v>-0.5894136629187723</v>
       </c>
       <c r="C5" t="n">
-        <v>1.097426557372159e-19</v>
+        <v>9.593915512202333e-13</v>
       </c>
     </row>
     <row r="6">
@@ -827,10 +814,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.1940762801218127</v>
+        <v>-0.1392439130416601</v>
       </c>
       <c r="C6" t="n">
-        <v>0.08356243776495302</v>
+        <v>0.2243846054048748</v>
       </c>
     </row>
     <row r="7">
@@ -840,10 +827,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.06722323415944671</v>
+        <v>0.0453368842970461</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1196171167574819</v>
+        <v>0.3281235179116698</v>
       </c>
     </row>
     <row r="8">
@@ -853,10 +840,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0002782781070856956</v>
+        <v>0.0003909880653039681</v>
       </c>
       <c r="C8" t="n">
-        <v>2.007195865076835e-55</v>
+        <v>3.081030640093266e-94</v>
       </c>
     </row>
     <row r="9">
@@ -866,10 +853,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.01960874951943636</v>
+        <v>0.02204055469398669</v>
       </c>
       <c r="C9" t="n">
-        <v>1.744864357214495e-26</v>
+        <v>1.112170525763271e-30</v>
       </c>
     </row>
     <row r="10">
@@ -879,10 +866,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.1664107630533422</v>
+        <v>-0.1994489392035889</v>
       </c>
       <c r="C10" t="n">
-        <v>0.001125157911111269</v>
+        <v>0.0001557593597625783</v>
       </c>
     </row>
     <row r="11">
@@ -892,10 +879,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.4058448968614469</v>
+        <v>0.4494066485643196</v>
       </c>
       <c r="C11" t="n">
-        <v>4.131788734638135e-07</v>
+        <v>4.709905613010037e-08</v>
       </c>
     </row>
     <row r="12">
@@ -905,10 +892,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3418067826769314</v>
+        <v>0.1623683855327539</v>
       </c>
       <c r="C12" t="n">
-        <v>0.000513903275130259</v>
+        <v>0.1097058341150496</v>
       </c>
     </row>
     <row r="13">
@@ -918,10 +905,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-7.332474611415027e-05</v>
+        <v>-7.973271875176693e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>5.012886850831805e-24</v>
+        <v>1.437196493504132e-26</v>
       </c>
     </row>
     <row r="14">
@@ -931,10 +918,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4.311469831398117e-09</v>
+        <v>8.35274708536417e-09</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7054412197187698</v>
+        <v>0.4543358410594162</v>
       </c>
     </row>
     <row r="15">
@@ -944,10 +931,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.006870342247563254</v>
+        <v>0.01653271847451401</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6701733830826047</v>
+        <v>0.3101665477472449</v>
       </c>
     </row>
     <row r="16">
@@ -957,10 +944,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07359770359897745</v>
+        <v>0.09160847163458759</v>
       </c>
       <c r="C16" t="n">
-        <v>1.878362222031774e-15</v>
+        <v>7.486805164528012e-27</v>
       </c>
     </row>
     <row r="17">
@@ -970,10 +957,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.3814087285159948</v>
+        <v>-0.16979601200813</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3321546363105182</v>
+        <v>0.6809993737546161</v>
       </c>
     </row>
     <row r="18">
@@ -983,23 +970,23 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.002783923003090526</v>
+        <v>0.0009903252676546394</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3280268762000876</v>
+        <v>0.7376275015189646</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.003350249551987248</v>
+        <v>0.002218221644631663</v>
       </c>
       <c r="C19" t="n">
-        <v>0.03140437615670362</v>
+        <v>0.164969902229695</v>
       </c>
     </row>
     <row r="20">
@@ -1009,10 +996,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.08511933604872</v>
+        <v>1.06020046881647</v>
       </c>
       <c r="C20" t="n">
-        <v>4.985538748800539e-06</v>
+        <v>6.328031998001885e-09</v>
       </c>
     </row>
     <row r="21">
@@ -1022,23 +1009,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.1328858987692287</v>
+        <v>-0.6928446115431917</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6569492037467328</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.4000623058994169</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.06284848039272241</v>
+        <v>0.01068119424755462</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1026,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1084,10 +1058,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.980369403495468</v>
+        <v>-2.443067941438994</v>
       </c>
       <c r="C2" t="n">
-        <v>8.179228347947119e-07</v>
+        <v>3.533124156529688e-12</v>
       </c>
     </row>
     <row r="3">
@@ -1097,10 +1071,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.125939328570613</v>
+        <v>0.2193925984539069</v>
       </c>
       <c r="C3" t="n">
-        <v>0.154537659384375</v>
+        <v>0.02088151468600644</v>
       </c>
     </row>
     <row r="4">
@@ -1110,10 +1084,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.168039847871428</v>
+        <v>-1.211100594690842</v>
       </c>
       <c r="C4" t="n">
-        <v>2.699410652468072e-52</v>
+        <v>6.775385255432841e-53</v>
       </c>
     </row>
     <row r="5">
@@ -1123,10 +1097,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.7625617387850488</v>
+        <v>-0.6722551963519175</v>
       </c>
       <c r="C5" t="n">
-        <v>1.455942268475826e-21</v>
+        <v>3.488193213113551e-16</v>
       </c>
     </row>
     <row r="6">
@@ -1136,10 +1110,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.2141403734356452</v>
+        <v>-0.1931118887302848</v>
       </c>
       <c r="C6" t="n">
-        <v>0.05071421129206916</v>
+        <v>0.08708829301756806</v>
       </c>
     </row>
     <row r="7">
@@ -1149,10 +1123,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.07939293848172695</v>
+        <v>0.02185881168871432</v>
       </c>
       <c r="C7" t="n">
-        <v>0.06258017033889687</v>
+        <v>0.6343253957508886</v>
       </c>
     </row>
     <row r="8">
@@ -1162,10 +1136,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0002843314878919213</v>
+        <v>0.0003889507803508715</v>
       </c>
       <c r="C8" t="n">
-        <v>6.571408772449514e-58</v>
+        <v>1.949433046159409e-92</v>
       </c>
     </row>
     <row r="9">
@@ -1175,10 +1149,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.01910960345934223</v>
+        <v>0.02292284308158045</v>
       </c>
       <c r="C9" t="n">
-        <v>5.114494861218358e-25</v>
+        <v>7.100231014857933e-33</v>
       </c>
     </row>
     <row r="10">
@@ -1188,10 +1162,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.2126808565012566</v>
+        <v>-0.1848864451716765</v>
       </c>
       <c r="C10" t="n">
-        <v>3.444416364144794e-05</v>
+        <v>0.0004805714907878909</v>
       </c>
     </row>
     <row r="11">
@@ -1201,10 +1175,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.4079014938029649</v>
+        <v>0.47403119590383</v>
       </c>
       <c r="C11" t="n">
-        <v>4.970758327297609e-07</v>
+        <v>1.03926918847397e-08</v>
       </c>
     </row>
     <row r="12">
@@ -1214,10 +1188,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3842079509342966</v>
+        <v>0.1620331774401659</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0001067675966789129</v>
+        <v>0.1121241370308716</v>
       </c>
     </row>
     <row r="13">
@@ -1227,10 +1201,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-6.897471059616255e-05</v>
+        <v>-8.766001575078295e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>1.313753400673464e-21</v>
+        <v>1.163653262137317e-31</v>
       </c>
     </row>
     <row r="14">
@@ -1240,10 +1214,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-3.579835208836353e-10</v>
+        <v>1.597451847459569e-08</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9747646769028557</v>
+        <v>0.1509056583981505</v>
       </c>
     </row>
     <row r="15">
@@ -1253,10 +1227,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.009870104287749881</v>
+        <v>0.01404288942914636</v>
       </c>
       <c r="C15" t="n">
-        <v>0.549054808951698</v>
+        <v>0.3916411494354353</v>
       </c>
     </row>
     <row r="16">
@@ -1266,10 +1240,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07798750481627301</v>
+        <v>0.08548561634399142</v>
       </c>
       <c r="C16" t="n">
-        <v>4.479632246995761e-17</v>
+        <v>2.302949240773119e-23</v>
       </c>
     </row>
     <row r="17">
@@ -1279,10 +1253,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.03445165692620997</v>
+        <v>-0.4465175301898216</v>
       </c>
       <c r="C17" t="n">
-        <v>0.9304052254211457</v>
+        <v>0.2785327567401366</v>
       </c>
     </row>
     <row r="18">
@@ -1292,23 +1266,23 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.0004970265459671119</v>
+        <v>0.0005992064434555452</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8614709257423259</v>
+        <v>0.8392968386303193</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.002686315031499509</v>
+        <v>0.002504191005896892</v>
       </c>
       <c r="C19" t="n">
-        <v>0.08482685823959271</v>
+        <v>0.1141523274983779</v>
       </c>
     </row>
     <row r="20">
@@ -1318,10 +1292,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.219262414646804</v>
+        <v>1.122500801341507</v>
       </c>
       <c r="C20" t="n">
-        <v>3.01644443852456e-07</v>
+        <v>8.65032044987982e-10</v>
       </c>
     </row>
     <row r="21">
@@ -1331,23 +1305,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.1174551358523414</v>
+        <v>-0.5558173185438446</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6958678525280779</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.4772291348141879</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.02668545084493079</v>
+        <v>0.04097373634201609</v>
       </c>
     </row>
   </sheetData>
@@ -1361,7 +1322,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1393,10 +1354,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.816666690373179</v>
+        <v>-2.656538252785407</v>
       </c>
       <c r="C2" t="n">
-        <v>6.08347001360474e-06</v>
+        <v>3.925387887652397e-14</v>
       </c>
     </row>
     <row r="3">
@@ -1406,10 +1367,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2301654919040214</v>
+        <v>0.2438634288164655</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01000263465733526</v>
+        <v>0.0102436332355551</v>
       </c>
     </row>
     <row r="4">
@@ -1419,10 +1380,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.188717204035874</v>
+        <v>-1.143465316958557</v>
       </c>
       <c r="C4" t="n">
-        <v>2.087442564568932e-54</v>
+        <v>3.899760266978024e-47</v>
       </c>
     </row>
     <row r="5">
@@ -1432,10 +1393,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.7728214068621225</v>
+        <v>-0.6056176262395561</v>
       </c>
       <c r="C5" t="n">
-        <v>2.78122466957847e-22</v>
+        <v>2.34395415434355e-13</v>
       </c>
     </row>
     <row r="6">
@@ -1445,10 +1406,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.1777307378335531</v>
+        <v>-0.184041875377383</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1083660802506915</v>
+        <v>0.1085042478683867</v>
       </c>
     </row>
     <row r="7">
@@ -1458,10 +1419,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.03536765555966251</v>
+        <v>0.0415363752877114</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4113690195523469</v>
+        <v>0.3652377952947832</v>
       </c>
     </row>
     <row r="8">
@@ -1471,10 +1432,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0002860018694054194</v>
+        <v>0.0003964702505693456</v>
       </c>
       <c r="C8" t="n">
-        <v>1.403545953218731e-58</v>
+        <v>2.350392632257859e-95</v>
       </c>
     </row>
     <row r="9">
@@ -1484,10 +1445,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.02022241974046066</v>
+        <v>0.02372980388769434</v>
       </c>
       <c r="C9" t="n">
-        <v>5.4285783082028e-28</v>
+        <v>3.38599480297491e-35</v>
       </c>
     </row>
     <row r="10">
@@ -1497,10 +1458,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.1970867765963544</v>
+        <v>-0.2139087972575423</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0001120189646536636</v>
+        <v>4.846730638590067e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1510,10 +1471,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3824139978098576</v>
+        <v>0.4390737602412353</v>
       </c>
       <c r="C11" t="n">
-        <v>2.287462602343315e-06</v>
+        <v>1.077934438757595e-07</v>
       </c>
     </row>
     <row r="12">
@@ -1523,10 +1484,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3342321265139644</v>
+        <v>0.1034585666053244</v>
       </c>
       <c r="C12" t="n">
-        <v>0.000689194165828236</v>
+        <v>0.3088764948299412</v>
       </c>
     </row>
     <row r="13">
@@ -1536,10 +1497,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-7.083533136258365e-05</v>
+        <v>-8.297543297845738e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>1.616840091331085e-22</v>
+        <v>1.309083935526002e-28</v>
       </c>
     </row>
     <row r="14">
@@ -1549,10 +1510,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-2.79177127184325e-10</v>
+        <v>1.465356889864606e-08</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9806932346932512</v>
+        <v>0.1863187827556883</v>
       </c>
     </row>
     <row r="15">
@@ -1562,10 +1523,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.006229938493742963</v>
+        <v>0.0182774382470505</v>
       </c>
       <c r="C15" t="n">
-        <v>0.703196911726204</v>
+        <v>0.2586491138758972</v>
       </c>
     </row>
     <row r="16">
@@ -1575,10 +1536,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07037350748308487</v>
+        <v>0.09308452350384169</v>
       </c>
       <c r="C16" t="n">
-        <v>3.163687083489718e-14</v>
+        <v>1.847864740429099e-27</v>
       </c>
     </row>
     <row r="17">
@@ -1588,10 +1549,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.06089892406108516</v>
+        <v>-0.1757978214264523</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8772625997099474</v>
+        <v>0.6715544090134629</v>
       </c>
     </row>
     <row r="18">
@@ -1601,23 +1562,23 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.001320873318220603</v>
+        <v>0.001841747802280817</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6428699483159126</v>
+        <v>0.5328221234725385</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.002811634931463216</v>
+        <v>0.002125137613601681</v>
       </c>
       <c r="C19" t="n">
-        <v>0.07137061768055186</v>
+        <v>0.1788105680873842</v>
       </c>
     </row>
     <row r="20">
@@ -1627,10 +1588,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.28228240116853</v>
+        <v>1.081729642156458</v>
       </c>
       <c r="C20" t="n">
-        <v>6.602710102902693e-08</v>
+        <v>2.525234387365951e-09</v>
       </c>
     </row>
     <row r="21">
@@ -1640,23 +1601,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.1287001683591534</v>
+        <v>-0.451034770177669</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6692097420562358</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.606433646386578</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.004956273373604779</v>
+        <v>0.09620257373880854</v>
       </c>
     </row>
   </sheetData>
@@ -1670,7 +1618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1702,10 +1650,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.794549253121291</v>
+        <v>-2.715421040648473</v>
       </c>
       <c r="C2" t="n">
-        <v>8.223520141602711e-06</v>
+        <v>1.668036840930238e-14</v>
       </c>
     </row>
     <row r="3">
@@ -1715,10 +1663,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1692379898621558</v>
+        <v>0.207738366799686</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05754087719964365</v>
+        <v>0.02898944907151853</v>
       </c>
     </row>
     <row r="4">
@@ -1728,10 +1676,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.135855605003109</v>
+        <v>-1.128424415586438</v>
       </c>
       <c r="C4" t="n">
-        <v>2.210370565941984e-49</v>
+        <v>5.445908738883908e-46</v>
       </c>
     </row>
     <row r="5">
@@ -1741,10 +1689,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.6973871684494017</v>
+        <v>-0.5867197961396677</v>
       </c>
       <c r="C5" t="n">
-        <v>2.562205425488756e-18</v>
+        <v>1.129257946467025e-12</v>
       </c>
     </row>
     <row r="6">
@@ -1754,10 +1702,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.2100245503931333</v>
+        <v>-0.2172910780675055</v>
       </c>
       <c r="C6" t="n">
-        <v>0.05905801060726448</v>
+        <v>0.05665119932076317</v>
       </c>
     </row>
     <row r="7">
@@ -1767,10 +1715,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.06809643459941493</v>
+        <v>0.05653353348476083</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1158536979271145</v>
+        <v>0.2218183625996893</v>
       </c>
     </row>
     <row r="8">
@@ -1780,10 +1728,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0002800863506110397</v>
+        <v>0.0003866231860319736</v>
       </c>
       <c r="C8" t="n">
-        <v>3.670249423822661e-56</v>
+        <v>7.049673224036546e-92</v>
       </c>
     </row>
     <row r="9">
@@ -1793,10 +1741,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.01944898080588794</v>
+        <v>0.02184218587149379</v>
       </c>
       <c r="C9" t="n">
-        <v>3.728589458982922e-26</v>
+        <v>3.371923510947477e-30</v>
       </c>
     </row>
     <row r="10">
@@ -1806,10 +1754,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.1666624195263811</v>
+        <v>-0.173912526663291</v>
       </c>
       <c r="C10" t="n">
-        <v>0.00110239792456419</v>
+        <v>0.000930372910717064</v>
       </c>
     </row>
     <row r="11">
@@ -1819,10 +1767,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3722358425549728</v>
+        <v>0.4475700401266511</v>
       </c>
       <c r="C11" t="n">
-        <v>3.525988477736432e-06</v>
+        <v>5.163756842117197e-08</v>
       </c>
     </row>
     <row r="12">
@@ -1832,10 +1780,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3504514833391781</v>
+        <v>0.1821640399468271</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0003634853296858923</v>
+        <v>0.07125572595619052</v>
       </c>
     </row>
     <row r="13">
@@ -1845,10 +1793,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-7.103961707161005e-05</v>
+        <v>-8.338276119422021e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>1.37820414005112e-22</v>
+        <v>3.522661310728859e-29</v>
       </c>
     </row>
     <row r="14">
@@ -1858,10 +1806,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-2.841859677492108e-09</v>
+        <v>1.331564207124297e-08</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8039495599870059</v>
+        <v>0.2197543688565904</v>
       </c>
     </row>
     <row r="15">
@@ -1871,10 +1819,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.0011641895942622</v>
+        <v>0.01332463011947367</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9430294314953924</v>
+        <v>0.4121021772219423</v>
       </c>
     </row>
     <row r="16">
@@ -1884,10 +1832,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07300002912283675</v>
+        <v>0.08753908751053621</v>
       </c>
       <c r="C16" t="n">
-        <v>4.889505875285364e-15</v>
+        <v>1.665525654582936e-24</v>
       </c>
     </row>
     <row r="17">
@@ -1897,10 +1845,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.136052463991979</v>
+        <v>-0.1548477184310048</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7288531258100872</v>
+        <v>0.7075731770997632</v>
       </c>
     </row>
     <row r="18">
@@ -1910,23 +1858,23 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.0006271235343535215</v>
+        <v>0.001758840877796799</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8258472036850451</v>
+        <v>0.5494587662343776</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.002651733507875734</v>
+        <v>0.003644642080507435</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0930750522550893</v>
+        <v>0.02342869342250322</v>
       </c>
     </row>
     <row r="20">
@@ -1936,10 +1884,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.193875013125902</v>
+        <v>1.1006180377867</v>
       </c>
       <c r="C20" t="n">
-        <v>5.182369179642809e-07</v>
+        <v>1.758776342653108e-09</v>
       </c>
     </row>
     <row r="21">
@@ -1949,23 +1897,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.1444825189167168</v>
+        <v>-0.5329128706470981</v>
       </c>
       <c r="C21" t="n">
-        <v>0.630447087159941</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.5446725871767807</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.0114320604491428</v>
+        <v>0.05048356551825958</v>
       </c>
     </row>
   </sheetData>
@@ -1979,7 +1914,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2011,10 +1946,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.888927677751125</v>
+        <v>-2.566295675054987</v>
       </c>
       <c r="C2" t="n">
-        <v>2.436035456756903e-06</v>
+        <v>2.70159641479666e-13</v>
       </c>
     </row>
     <row r="3">
@@ -2024,10 +1959,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1296510920848891</v>
+        <v>0.2168428410777438</v>
       </c>
       <c r="C3" t="n">
-        <v>0.143284349133897</v>
+        <v>0.02265340129680423</v>
       </c>
     </row>
     <row r="4">
@@ -2037,10 +1972,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.172829019807213</v>
+        <v>-1.147515270914539</v>
       </c>
       <c r="C4" t="n">
-        <v>6.711062311427771e-53</v>
+        <v>7.083285493821616e-48</v>
       </c>
     </row>
     <row r="5">
@@ -2050,10 +1985,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.7161764356705228</v>
+        <v>-0.5987400949692948</v>
       </c>
       <c r="C5" t="n">
-        <v>2.037258010260989e-19</v>
+        <v>3.422055005893417e-13</v>
       </c>
     </row>
     <row r="6">
@@ -2063,10 +1998,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.191300868402096</v>
+        <v>-0.2210864266366179</v>
       </c>
       <c r="C6" t="n">
-        <v>0.08464087126983297</v>
+        <v>0.05056239126031085</v>
       </c>
     </row>
     <row r="7">
@@ -2076,10 +2011,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.06174046661076569</v>
+        <v>0.04377839843754557</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1492230428633003</v>
+        <v>0.3410552947076583</v>
       </c>
     </row>
     <row r="8">
@@ -2089,10 +2024,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0003041822219770333</v>
+        <v>0.0003869287959769364</v>
       </c>
       <c r="C8" t="n">
-        <v>1.76256631343902e-65</v>
+        <v>1.023495168090521e-92</v>
       </c>
     </row>
     <row r="9">
@@ -2102,10 +2037,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.01969033950197499</v>
+        <v>0.02375975436995684</v>
       </c>
       <c r="C9" t="n">
-        <v>1.891960054452844e-26</v>
+        <v>2.902513118794997e-35</v>
       </c>
     </row>
     <row r="10">
@@ -2115,10 +2050,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.1803390887590847</v>
+        <v>-0.2044322262309794</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0004251092400172026</v>
+        <v>9.4112132815702e-05</v>
       </c>
     </row>
     <row r="11">
@@ -2128,10 +2063,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3764349662277631</v>
+        <v>0.4025327544913608</v>
       </c>
       <c r="C11" t="n">
-        <v>3.146192956943224e-06</v>
+        <v>1.183357684063432e-06</v>
       </c>
     </row>
     <row r="12">
@@ -2141,10 +2076,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3190046294090331</v>
+        <v>0.05312565103239545</v>
       </c>
       <c r="C12" t="n">
-        <v>0.001228195173176212</v>
+        <v>0.6020626737127797</v>
       </c>
     </row>
     <row r="13">
@@ -2154,10 +2089,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-7.810443957668597e-05</v>
+        <v>-8.025944736063299e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>5.930278891807778e-27</v>
+        <v>3.027295972031442e-27</v>
       </c>
     </row>
     <row r="14">
@@ -2167,10 +2102,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>8.068521925445036e-09</v>
+        <v>1.467843266160708e-08</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4792810357433934</v>
+        <v>0.1783138254827682</v>
       </c>
     </row>
     <row r="15">
@@ -2180,10 +2115,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.001893644499184058</v>
+        <v>0.02118492896925245</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9072001098404934</v>
+        <v>0.1910279719951136</v>
       </c>
     </row>
     <row r="16">
@@ -2193,10 +2128,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07218474446448843</v>
+        <v>0.08894491790293078</v>
       </c>
       <c r="C16" t="n">
-        <v>6.059264302247756e-15</v>
+        <v>2.36977478279083e-25</v>
       </c>
     </row>
     <row r="17">
@@ -2206,10 +2141,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.5057579655779406</v>
+        <v>-0.4570747134973325</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1974056582045028</v>
+        <v>0.2588345948288412</v>
       </c>
     </row>
     <row r="18">
@@ -2219,23 +2154,23 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.0004680726292803492</v>
+        <v>0.001633765246986096</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8695979419748516</v>
+        <v>0.5773955822412579</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.003000982031114473</v>
+        <v>0.002387906974207621</v>
       </c>
       <c r="C19" t="n">
-        <v>0.05452577523574117</v>
+        <v>0.1349875827262561</v>
       </c>
     </row>
     <row r="20">
@@ -2245,10 +2180,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.301098775742336</v>
+        <v>1.033812922493045</v>
       </c>
       <c r="C20" t="n">
-        <v>4.67298925913626e-08</v>
+        <v>1.16150427096327e-08</v>
       </c>
     </row>
     <row r="21">
@@ -2258,23 +2193,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.2437019376287906</v>
+        <v>-0.5303313748178343</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4181795666283172</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.5181449034262671</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.01600691673418356</v>
+        <v>0.05107336955338133</v>
       </c>
     </row>
   </sheetData>
@@ -2288,7 +2210,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2320,10 +2242,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-2.035019010823263</v>
+        <v>-2.556424953531254</v>
       </c>
       <c r="C2" t="n">
-        <v>3.701310479736041e-07</v>
+        <v>5.439432792190029e-13</v>
       </c>
     </row>
     <row r="3">
@@ -2333,10 +2255,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1396942698602518</v>
+        <v>0.2074320093468782</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1178377127234301</v>
+        <v>0.03023211364474166</v>
       </c>
     </row>
     <row r="4">
@@ -2346,10 +2268,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.10840004529217</v>
+        <v>-1.150771649967118</v>
       </c>
       <c r="C4" t="n">
-        <v>9.798838113784305e-48</v>
+        <v>5.992278007417019e-48</v>
       </c>
     </row>
     <row r="5">
@@ -2359,10 +2281,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.6734511122032093</v>
+        <v>-0.626957724752278</v>
       </c>
       <c r="C5" t="n">
-        <v>3.071722618053411e-17</v>
+        <v>4.035523984007086e-14</v>
       </c>
     </row>
     <row r="6">
@@ -2372,10 +2294,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.1176381313495237</v>
+        <v>-0.2773629963866648</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2910306969645816</v>
+        <v>0.01471534744449566</v>
       </c>
     </row>
     <row r="7">
@@ -2385,10 +2307,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.07477483301901079</v>
+        <v>0.0554936461818191</v>
       </c>
       <c r="C7" t="n">
-        <v>0.08280621429210892</v>
+        <v>0.2325103873846021</v>
       </c>
     </row>
     <row r="8">
@@ -2398,10 +2320,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0002995880175045746</v>
+        <v>0.0003807424253691289</v>
       </c>
       <c r="C8" t="n">
-        <v>4.991612671812014e-63</v>
+        <v>2.918025419779418e-90</v>
       </c>
     </row>
     <row r="9">
@@ -2411,10 +2333,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.01953727218020512</v>
+        <v>0.0223145893379422</v>
       </c>
       <c r="C9" t="n">
-        <v>2.122181797151363e-26</v>
+        <v>1.759596385286907e-31</v>
       </c>
     </row>
     <row r="10">
@@ -2424,10 +2346,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.1920240547265785</v>
+        <v>-0.2067361867212802</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0001654748146344203</v>
+        <v>8.30457288763907e-05</v>
       </c>
     </row>
     <row r="11">
@@ -2437,10 +2359,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3977085326166064</v>
+        <v>0.4330846741711058</v>
       </c>
       <c r="C11" t="n">
-        <v>7.610134786594857e-07</v>
+        <v>1.617610260849181e-07</v>
       </c>
     </row>
     <row r="12">
@@ -2450,10 +2372,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3549352609957711</v>
+        <v>0.1360520422295131</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0003041244516859464</v>
+        <v>0.1824631521704299</v>
       </c>
     </row>
     <row r="13">
@@ -2463,10 +2385,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-7.114919378757528e-05</v>
+        <v>-8.295281794137792e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>1.321426437301633e-22</v>
+        <v>7.695089921652094e-29</v>
       </c>
     </row>
     <row r="14">
@@ -2476,10 +2398,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-3.820757728360132e-10</v>
+        <v>2.033187080390648e-08</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9732552975618158</v>
+        <v>0.06501687367914524</v>
       </c>
     </row>
     <row r="15">
@@ -2489,10 +2411,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.01654742731206471</v>
+        <v>0.01401363935346244</v>
       </c>
       <c r="C15" t="n">
-        <v>0.3123487556565275</v>
+        <v>0.3910732147526131</v>
       </c>
     </row>
     <row r="16">
@@ -2502,10 +2424,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07124617326601794</v>
+        <v>0.09211889353311377</v>
       </c>
       <c r="C16" t="n">
-        <v>1.549570987558707e-14</v>
+        <v>6.257423986398563e-27</v>
       </c>
     </row>
     <row r="17">
@@ -2515,10 +2437,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.4045068244233698</v>
+        <v>-0.117119070250672</v>
       </c>
       <c r="C17" t="n">
-        <v>0.301630963149436</v>
+        <v>0.7773770454766843</v>
       </c>
     </row>
     <row r="18">
@@ -2528,23 +2450,23 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.001610289373250594</v>
+        <v>0.001276800295351474</v>
       </c>
       <c r="C18" t="n">
-        <v>0.5717201132595978</v>
+        <v>0.6659539357679705</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.003195818456806365</v>
+        <v>0.002829500064808607</v>
       </c>
       <c r="C19" t="n">
-        <v>0.03973969120670891</v>
+        <v>0.08224094435981369</v>
       </c>
     </row>
     <row r="20">
@@ -2554,10 +2476,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.141874794418253</v>
+        <v>1.019510693018933</v>
       </c>
       <c r="C20" t="n">
-        <v>1.679452717331794e-06</v>
+        <v>2.397620502499749e-08</v>
       </c>
     </row>
     <row r="21">
@@ -2567,23 +2489,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.0892431109383999</v>
+        <v>-0.7912433267889628</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7671834404799397</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.4880458119459786</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.02354724866871515</v>
+        <v>0.003542807754565457</v>
       </c>
     </row>
   </sheetData>
@@ -2597,7 +2506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2629,10 +2538,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.756318731189601</v>
+        <v>-2.668573134288743</v>
       </c>
       <c r="C2" t="n">
-        <v>1.244242322956687e-05</v>
+        <v>3.530101931531714e-14</v>
       </c>
     </row>
     <row r="3">
@@ -2642,10 +2551,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1884469115088475</v>
+        <v>0.1595737273991206</v>
       </c>
       <c r="C3" t="n">
-        <v>0.03433009385215052</v>
+        <v>0.09775702095499644</v>
       </c>
     </row>
     <row r="4">
@@ -2655,10 +2564,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.17217367507538</v>
+        <v>-1.093437311584253</v>
       </c>
       <c r="C4" t="n">
-        <v>8.562216295603887e-53</v>
+        <v>2.583389781702571e-42</v>
       </c>
     </row>
     <row r="5">
@@ -2668,10 +2577,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.763192139889155</v>
+        <v>-0.5409449955471745</v>
       </c>
       <c r="C5" t="n">
-        <v>1.029127965248077e-21</v>
+        <v>9.114145549618739e-11</v>
       </c>
     </row>
     <row r="6">
@@ -2681,10 +2590,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.1955862652577282</v>
+        <v>-0.1717039385988876</v>
       </c>
       <c r="C6" t="n">
-        <v>0.07711550006134077</v>
+        <v>0.1328251132575678</v>
       </c>
     </row>
     <row r="7">
@@ -2694,10 +2603,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0569184711178163</v>
+        <v>0.09230699033484531</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1848176599364294</v>
+        <v>0.05184167142125768</v>
       </c>
     </row>
     <row r="8">
@@ -2707,10 +2616,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0002912845969901456</v>
+        <v>0.0003857697073102555</v>
       </c>
       <c r="C8" t="n">
-        <v>1.879781322377574e-60</v>
+        <v>1.283568315665113e-91</v>
       </c>
     </row>
     <row r="9">
@@ -2720,10 +2629,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.01973451744234631</v>
+        <v>0.02336038645906733</v>
       </c>
       <c r="C9" t="n">
-        <v>7.950194323697211e-27</v>
+        <v>2.261235631404683e-34</v>
       </c>
     </row>
     <row r="10">
@@ -2733,10 +2642,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.1803698516697025</v>
+        <v>-0.2112378174159826</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0004328155862159895</v>
+        <v>6.197638932155549e-05</v>
       </c>
     </row>
     <row r="11">
@@ -2746,10 +2655,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.3704951616362588</v>
+        <v>0.4241208351740008</v>
       </c>
       <c r="C11" t="n">
-        <v>4.488827698066192e-06</v>
+        <v>2.480928698824709e-07</v>
       </c>
     </row>
     <row r="12">
@@ -2759,10 +2668,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3200193241865491</v>
+        <v>0.1163001639277524</v>
       </c>
       <c r="C12" t="n">
-        <v>0.001215670871246287</v>
+        <v>0.2494986668993959</v>
       </c>
     </row>
     <row r="13">
@@ -2772,10 +2681,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-6.893455553048796e-05</v>
+        <v>-7.882112879522959e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>1.968489939877159e-21</v>
+        <v>3.485343463997295e-26</v>
       </c>
     </row>
     <row r="14">
@@ -2785,10 +2694,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-2.778471191594816e-10</v>
+        <v>2.754053921444435e-09</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9803775129870815</v>
+        <v>0.8002823990456578</v>
       </c>
     </row>
     <row r="15">
@@ -2798,10 +2707,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.001592588594433718</v>
+        <v>0.01922578744002221</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9217874231631122</v>
+        <v>0.2359217674317138</v>
       </c>
     </row>
     <row r="16">
@@ -2811,10 +2720,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07722605622114027</v>
+        <v>0.08308477873884547</v>
       </c>
       <c r="C16" t="n">
-        <v>1.212115704445158e-16</v>
+        <v>2.47598486156335e-22</v>
       </c>
     </row>
     <row r="17">
@@ -2824,10 +2733,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.310583552603203</v>
+        <v>-0.400477726221502</v>
       </c>
       <c r="C17" t="n">
-        <v>0.4334180190843199</v>
+        <v>0.3284946089846201</v>
       </c>
     </row>
     <row r="18">
@@ -2837,23 +2746,23 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>8.233334451837954e-05</v>
+        <v>0.002999009868709332</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9770462606809661</v>
+        <v>0.3082129133310448</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.001883180431021225</v>
+        <v>0.002957690587322866</v>
       </c>
       <c r="C19" t="n">
-        <v>0.2307603422727998</v>
+        <v>0.06392804904576783</v>
       </c>
     </row>
     <row r="20">
@@ -2863,10 +2772,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.161611245419881</v>
+        <v>1.013723151241701</v>
       </c>
       <c r="C20" t="n">
-        <v>1.066902922562088e-06</v>
+        <v>2.743915382145499e-08</v>
       </c>
     </row>
     <row r="21">
@@ -2876,23 +2785,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.1614789907915427</v>
+        <v>-0.6067851910501665</v>
       </c>
       <c r="C21" t="n">
-        <v>0.5906379258755456</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.4833482136245835</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.02489822976560332</v>
+        <v>0.02541125371157595</v>
       </c>
     </row>
   </sheetData>
@@ -2906,7 +2802,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2938,10 +2834,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-1.979543335721889</v>
+        <v>-2.623720031206609</v>
       </c>
       <c r="C2" t="n">
-        <v>8.074449196414448e-07</v>
+        <v>6.064246747736109e-14</v>
       </c>
     </row>
     <row r="3">
@@ -2951,10 +2847,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1154346233662818</v>
+        <v>0.2698726475322406</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1959645114689361</v>
+        <v>0.004479496754670582</v>
       </c>
     </row>
     <row r="4">
@@ -2964,10 +2860,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.171615535047153</v>
+        <v>-1.116896553190033</v>
       </c>
       <c r="C4" t="n">
-        <v>7.732079500999084e-53</v>
+        <v>2.384187755542328e-45</v>
       </c>
     </row>
     <row r="5">
@@ -2977,10 +2873,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.7442556802626554</v>
+        <v>-0.6075151711043605</v>
       </c>
       <c r="C5" t="n">
-        <v>1.246297807577603e-20</v>
+        <v>1.66777450471327e-13</v>
       </c>
     </row>
     <row r="6">
@@ -2990,10 +2886,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.2779646415119025</v>
+        <v>-0.1823557814035307</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01287009397903039</v>
+        <v>0.1056900349754599</v>
       </c>
     </row>
     <row r="7">
@@ -3003,10 +2899,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.07673101077146259</v>
+        <v>0.03725501094812891</v>
       </c>
       <c r="C7" t="n">
-        <v>0.07488175855641735</v>
+        <v>0.4174323042050011</v>
       </c>
     </row>
     <row r="8">
@@ -3016,10 +2912,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0002904978394850484</v>
+        <v>0.00039077124555368</v>
       </c>
       <c r="C8" t="n">
-        <v>4.233105545456869e-60</v>
+        <v>1.826383205986508e-93</v>
       </c>
     </row>
     <row r="9">
@@ -3029,10 +2925,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.01913260666884049</v>
+        <v>0.02283589438324836</v>
       </c>
       <c r="C9" t="n">
-        <v>2.674106835763898e-25</v>
+        <v>1.054874858934747e-32</v>
       </c>
     </row>
     <row r="10">
@@ -3042,10 +2938,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.172012181102874</v>
+        <v>-0.208702677485303</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0007643321795503141</v>
+        <v>7.209563113233973e-05</v>
       </c>
     </row>
     <row r="11">
@@ -3055,10 +2951,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.377370281714108</v>
+        <v>0.4479023099118123</v>
       </c>
       <c r="C11" t="n">
-        <v>3.464506447382808e-06</v>
+        <v>5.086253064121706e-08</v>
       </c>
     </row>
     <row r="12">
@@ -3068,10 +2964,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3502760612188163</v>
+        <v>0.1234974491071228</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0004189260666499519</v>
+        <v>0.2221485205386665</v>
       </c>
     </row>
     <row r="13">
@@ -3081,10 +2977,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-7.117257507439592e-05</v>
+        <v>-8.722097302187944e-05</v>
       </c>
       <c r="C13" t="n">
-        <v>1.398337953729173e-22</v>
+        <v>2.081415025732152e-31</v>
       </c>
     </row>
     <row r="14">
@@ -3094,10 +2990,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-1.787182747033854e-09</v>
+        <v>1.952545383560108e-08</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8762959928811969</v>
+        <v>0.0739740701428263</v>
       </c>
     </row>
     <row r="15">
@@ -3107,10 +3003,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.006303842358572291</v>
+        <v>0.01669706787648588</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6998655336316588</v>
+        <v>0.3075846392342779</v>
       </c>
     </row>
     <row r="16">
@@ -3120,10 +3016,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07441240858208409</v>
+        <v>0.09306313885215971</v>
       </c>
       <c r="C16" t="n">
-        <v>1.137336884851234e-15</v>
+        <v>1.402937592184329e-27</v>
       </c>
     </row>
     <row r="17">
@@ -3133,10 +3029,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.1489211956466299</v>
+        <v>-0.2241031990706943</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7070990225900775</v>
+        <v>0.58619666253185</v>
       </c>
     </row>
     <row r="18">
@@ -3146,23 +3042,23 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.002078343151569278</v>
+        <v>0.003441707031484558</v>
       </c>
       <c r="C18" t="n">
-        <v>0.4661951112713931</v>
+        <v>0.2424115718336546</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>StreetLength</t>
+          <t>street_length</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.002751239526797696</v>
+        <v>0.002428629309689556</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0782989494590115</v>
+        <v>0.1227907419788659</v>
       </c>
     </row>
     <row r="20">
@@ -3172,10 +3068,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1.225035677823444</v>
+        <v>1.015212709417511</v>
       </c>
       <c r="C20" t="n">
-        <v>2.530480235821477e-07</v>
+        <v>2.808827601656485e-08</v>
       </c>
     </row>
     <row r="21">
@@ -3185,23 +3081,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.07666908678146904</v>
+        <v>-0.5405181359682978</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7980821959276838</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LU_Urban</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>-0.484453653217824</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.02427545139368116</v>
+        <v>0.04526310720878404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>